<commit_message>
set y-axis to 0 on all plots
</commit_message>
<xml_diff>
--- a/Lettuce_Growth_Days/lettuce_EDA.xlsx
+++ b/Lettuce_Growth_Days/lettuce_EDA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2147105s_student_gla_ac_uk/Documents/Data_Analysis_Portfolio/Google_Data_Analytics_Certificate/Lettuce_Growth_Days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C858448F-821B-49A2-B533-580762CBF931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:40009_{C858448F-821B-49A2-B533-580762CBF931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BC95263-89C2-4C94-B05E-4FFEF878B7DF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lettuce_dataset" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -125,9 +138,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="mmmm"/>
+    <numFmt numFmtId="164" formatCode="mmmm"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -639,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1402,7 +1415,7 @@
         <c:axId val="304273807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="40"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1515,7 +1528,7 @@
         <c:crossAx val="124997215"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2264,7 +2277,7 @@
         <c:axId val="1425871311"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="40"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2377,7 +2390,8 @@
         <c:crossAx val="1022324575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="10"/>
+        <c:minorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3126,7 +3140,8 @@
         <c:axId val="1017143343"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="40"/>
+          <c:max val="70"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3992,7 +4007,7 @@
         <c:axId val="1418121759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="40"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6831,7 +6846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J3203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -80516,27 +80531,27 @@
         <v>8</v>
       </c>
       <c r="B3203" s="8">
-        <f>MIN(B2:B3196)</f>
+        <f t="shared" ref="B3203:G3203" si="5">MIN(B2:B3196)</f>
         <v>45141</v>
       </c>
       <c r="C3203" s="9">
-        <f>MIN(C2:C3196)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D3203" s="9">
-        <f>MIN(D2:D3196)</f>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="E3203" s="9">
-        <f>MIN(E2:E3196)</f>
+        <f t="shared" si="5"/>
         <v>400</v>
       </c>
       <c r="F3203" s="9">
-        <f>MIN(F2:F3196)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G3203" s="9">
-        <f>MIN(G2:G3196)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -80550,12 +80565,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>